<commit_message>
convert floats do decimals to comply with dynamodb requirements
</commit_message>
<xml_diff>
--- a/lib/tests/test_with_existing_config_sheet.xlsx
+++ b/lib/tests/test_with_existing_config_sheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="17604" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="17610" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -416,63 +416,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -490,13 +490,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -522,7 +522,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -548,7 +548,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -574,7 +574,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>

</xml_diff>